<commit_message>
commit thông báo thuê đất trả tiền 1 lần
</commit_message>
<xml_diff>
--- a/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoQuyetDinhMienTienThueDat.xlsx
+++ b/QuanLyThueDat.WebApp/Assets/Template/MauBaoCaoQuyetDinhMienTienThueDat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VNPT\QuanLyThueDat\QuanLyThueDat\QuanLyThueDat.WebApp\Assets\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458F06EE-6ECA-4334-9DD8-A7A334CB6867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3C5A50-3F1E-4A73-9D4F-22862FA04392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>UBND TỈNH NGHỆ AN</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Mã số thuế</t>
+  </si>
+  <si>
+    <t>Địa chỉ thửa đất</t>
   </si>
 </sst>
 </file>
@@ -522,64 +525,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="55.140625" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="3" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="1"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -589,8 +595,9 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -600,57 +607,62 @@
       <c r="C5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="K5:K6"/>
+  <mergeCells count="10">
+    <mergeCell ref="L5:L6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>